<commit_message>
Send message script committed
</commit_message>
<xml_diff>
--- a/SocialMedia/Data/Book2.xlsx
+++ b/SocialMedia/Data/Book2.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanpri\git\SocialMedia\SocialMedia\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456944AF-CC30-4EDF-9698-83F53F42516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14350" windowHeight="3800" activeTab="1"/>
+    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Test_ID</t>
   </si>
@@ -48,12 +53,18 @@
   </si>
   <si>
     <t>demo7184</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Hello</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -364,21 +375,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.08984375" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,7 +403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -412,29 +423,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>